<commit_message>
lock some rows and collums
</commit_message>
<xml_diff>
--- a/file/format.xlsx
+++ b/file/format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SimPerpus SMK Muh 1 Surakarta\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0985008-F075-4720-929B-7641DD82234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8715431-5D55-4901-8BC2-C7D94EBF7B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="2670" windowWidth="21600" windowHeight="11385" xr2:uid="{D7334611-F76B-409F-8608-5787832B01B8}"/>
+    <workbookView xWindow="2580" yWindow="2790" windowWidth="21600" windowHeight="11385" xr2:uid="{D7334611-F76B-409F-8608-5787832B01B8}"/>
   </bookViews>
   <sheets>
     <sheet name="anggota" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>nomor_anggota</t>
   </si>
@@ -76,58 +76,40 @@
     <t>Tri Kusmantoro</t>
   </si>
   <si>
-    <t>Eka Putri</t>
-  </si>
-  <si>
-    <t>Haryanto</t>
-  </si>
-  <si>
-    <t>Joko Adi Santoso</t>
-  </si>
-  <si>
-    <t>Senin bin Kamis</t>
-  </si>
-  <si>
-    <t>Isnan Nugroho</t>
-  </si>
-  <si>
-    <t>Adi Yahya Setiono</t>
-  </si>
-  <si>
     <t>siswa</t>
   </si>
   <si>
     <t>angkatan</t>
   </si>
   <si>
-    <t>md5(ubahyah1)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah2)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah3)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah4)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah5)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah6)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah7)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah8)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah9)</t>
-  </si>
-  <si>
-    <t>md5(ubahyah0)</t>
+    <t>ubahyah1</t>
+  </si>
+  <si>
+    <t>ubahyah2</t>
+  </si>
+  <si>
+    <t>ubahyah3</t>
+  </si>
+  <si>
+    <t>ubahyah4</t>
+  </si>
+  <si>
+    <t>ubahyah5</t>
+  </si>
+  <si>
+    <t>ubahyah6</t>
+  </si>
+  <si>
+    <t>ubahyah7</t>
+  </si>
+  <si>
+    <t>ubahyah8</t>
+  </si>
+  <si>
+    <t>ubahyah9</t>
+  </si>
+  <si>
+    <t>ubahyah10</t>
   </si>
 </sst>
 </file>
@@ -491,7 +473,8 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +497,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -528,13 +511,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>2019</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,13 +528,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
         <v>2019</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -562,13 +545,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>2019</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,13 +562,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>2019</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -596,13 +579,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,13 +596,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>2019</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -630,13 +613,13 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>2019</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -647,13 +630,13 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
         <v>2019</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,13 +647,13 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1">
         <v>2019</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,116 +664,56 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1">
         <v>2019</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>19106050011</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>19106050012</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>19106050013</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>19106050014</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>19106050015</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>19106050016</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -823,5 +746,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>